<commit_message>
Compil - corrections staff et locaux
</commit_message>
<xml_diff>
--- a/excel/locaux.xlsx
+++ b/excel/locaux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91BEDD86-3CEE-1E42-A75E-009AFCA7AA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC78B5A-E6CB-244C-9BC7-460F4F65D059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="560" windowWidth="23480" windowHeight="20380" activeTab="1" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>Salon VIP</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>Rencontres techniques</t>
+  </si>
+  <si>
+    <t>Material deposit - Neutral support</t>
+  </si>
+  <si>
+    <t>Dépôt de matérie -  Dépannage neutre</t>
   </si>
 </sst>
 </file>
@@ -711,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DDE1C1D-3050-7F46-8ECF-3B76DBA9970E}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,8 +1029,20 @@
         <v>1006 B</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="6" t="str">
+        <f t="shared" ref="D21" si="1">C21</f>
+        <v>TBD</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>

</xml_diff>